<commit_message>
Updated the price list and created a "release" version for the rest of the world (without inventory)
</commit_message>
<xml_diff>
--- a/ChaprSVN/PriceSourceList v3.xlsx
+++ b/ChaprSVN/PriceSourceList v3.xlsx
@@ -7,9 +7,7 @@
     <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10545"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Parts List" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -1654,28 +1652,4 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="64" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added the inventory, Presentation for Patent Signing.pptx and a picture of all the places the ChapR has been shipped too.
</commit_message>
<xml_diff>
--- a/ChaprSVN/PriceSourceList v3.xlsx
+++ b/ChaprSVN/PriceSourceList v3.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10545"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="20730" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Parts List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
   <si>
     <t>Part Name</t>
   </si>
@@ -274,9 +274,6 @@
     <t>- FMW part 1556.440316.188, 4-40 x 3/16 Phillips Pan Machine Screw 18-8 SS</t>
   </si>
   <si>
-    <t>misc (headers, label…)</t>
-  </si>
-  <si>
     <r>
       <t>24 k</t>
     </r>
@@ -326,22 +323,33 @@
     <t>Inventory as of</t>
   </si>
   <si>
-    <t>many</t>
-  </si>
-  <si>
-    <t>10 sets</t>
+    <t>100-200</t>
+  </si>
+  <si>
+    <t>approx. 100</t>
+  </si>
+  <si>
+    <t>100s</t>
+  </si>
+  <si>
+    <t>2 pins</t>
+  </si>
+  <si>
+    <t>6 pins</t>
+  </si>
+  <si>
+    <t>12 pins</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,6 +431,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -459,16 +474,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -476,14 +490,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -503,7 +514,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -517,11 +528,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -609,7 +623,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -644,7 +657,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -820,17 +832,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:L37"/>
+  <dimension ref="B2:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" customWidth="1"/>
@@ -842,89 +854,89 @@
     <col min="12" max="12" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F2" s="25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+    <row r="2" spans="2:12">
+      <c r="F2" s="22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="26">
-        <v>41618</v>
-      </c>
-      <c r="G3" s="16" t="s">
+      <c r="F3" s="23">
+        <v>41688</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="B4" s="5">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>27.05</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="6">
         <f>D4*B4</f>
         <v>27.05</v>
       </c>
-      <c r="F4" s="27">
-        <v>0</v>
-      </c>
-      <c r="G4" s="14" t="s">
+      <c r="F4" s="26">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11" t="s">
         <v>35</v>
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="6">
         <v>15.95</v>
       </c>
-      <c r="E5" s="1">
-        <f t="shared" ref="E5:E28" si="0">D5*B5</f>
+      <c r="E5" s="6">
+        <f t="shared" ref="E5:E30" si="0">D5*B5</f>
         <v>15.95</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="26">
         <v>0</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -938,11 +950,11 @@
       <c r="K5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -952,12 +964,12 @@
       <c r="D6" s="6">
         <v>8.9600000000000009</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <f t="shared" si="0"/>
         <v>8.9600000000000009</v>
       </c>
-      <c r="F6" s="27">
-        <v>9</v>
+      <c r="F6" s="26">
+        <v>0</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -966,9 +978,9 @@
         <v>28</v>
       </c>
       <c r="K6" s="4"/>
-      <c r="L6" s="21"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="18"/>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" s="5">
         <v>1</v>
       </c>
@@ -978,12 +990,12 @@
       <c r="D7" s="6">
         <v>0.09</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="F7" s="27" t="s">
-        <v>85</v>
+      <c r="F7" s="24">
+        <v>66</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>62</v>
@@ -992,9 +1004,9 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="22"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="2:12">
       <c r="B8" s="5">
         <v>1</v>
       </c>
@@ -1004,12 +1016,12 @@
       <c r="D8" s="6">
         <v>0.78</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="6">
         <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
-      <c r="F8" s="27">
-        <v>0</v>
+      <c r="F8" s="26">
+        <v>2</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>63</v>
@@ -1018,9 +1030,9 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="19"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="16"/>
+    </row>
+    <row r="9" spans="2:12">
       <c r="B9" s="5">
         <v>1</v>
       </c>
@@ -1030,12 +1042,12 @@
       <c r="D9" s="6">
         <v>0.3</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="6">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="F9" s="27" t="s">
-        <v>85</v>
+      <c r="F9" s="24">
+        <v>66</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1044,9 +1056,9 @@
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="22"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="19"/>
+    </row>
+    <row r="10" spans="2:12">
       <c r="B10" s="5">
         <v>1</v>
       </c>
@@ -1056,12 +1068,12 @@
       <c r="D10" s="6">
         <v>6.8</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="6">
         <f t="shared" si="0"/>
         <v>6.8</v>
       </c>
-      <c r="F10" s="27">
-        <v>2</v>
+      <c r="F10" s="24">
+        <v>33</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>41</v>
@@ -1070,11 +1082,11 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12">
       <c r="B11" s="5">
         <v>1</v>
       </c>
@@ -1084,12 +1096,12 @@
       <c r="D11" s="6">
         <v>0.25</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="6">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="F11" s="27">
-        <v>32</v>
+      <c r="F11" s="24">
+        <v>5</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>70</v>
@@ -1100,11 +1112,11 @@
         <v>37</v>
       </c>
       <c r="K11" s="4"/>
-      <c r="L11" s="19" t="s">
+      <c r="L11" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" s="5">
         <v>1</v>
       </c>
@@ -1114,23 +1126,23 @@
       <c r="D12" s="6">
         <v>7</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F12" s="27">
-        <v>10</v>
+      <c r="F12" s="26">
+        <v>0</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" s="5">
         <v>1</v>
       </c>
@@ -1140,11 +1152,11 @@
       <c r="D13" s="6">
         <v>0.99</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="6">
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="26">
         <v>0</v>
       </c>
       <c r="G13" s="4" t="s">
@@ -1154,9 +1166,9 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="19"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="16"/>
+    </row>
+    <row r="14" spans="2:12">
       <c r="B14" s="5">
         <v>1</v>
       </c>
@@ -1166,11 +1178,11 @@
       <c r="D14" s="6">
         <v>0.99</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="6">
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="26">
         <v>0</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -1182,11 +1194,11 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="19" t="s">
+      <c r="L14" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="B15" s="5">
         <v>4</v>
       </c>
@@ -1196,12 +1208,12 @@
       <c r="D15" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="6">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="F15" s="27" t="s">
-        <v>85</v>
+      <c r="F15" s="24" t="s">
+        <v>86</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>39</v>
@@ -1210,9 +1222,9 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="23"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="20"/>
+    </row>
+    <row r="16" spans="2:12">
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -1222,12 +1234,12 @@
       <c r="D16" s="6">
         <v>1.9E-2</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="6">
         <f t="shared" si="0"/>
         <v>0.13300000000000001</v>
       </c>
-      <c r="F16" s="27" t="s">
-        <v>85</v>
+      <c r="F16" s="24" t="s">
+        <v>86</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>68</v>
@@ -1236,35 +1248,35 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="23"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L16" s="20"/>
+    </row>
+    <row r="17" spans="2:12">
       <c r="B17" s="5">
         <v>1</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="6">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F17" s="27" t="s">
-        <v>85</v>
+      <c r="F17" s="24" t="s">
+        <v>84</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="23"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="20"/>
+    </row>
+    <row r="18" spans="2:12">
       <c r="B18" s="5">
         <v>2</v>
       </c>
@@ -1274,75 +1286,75 @@
       <c r="D18" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="6">
         <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="24" t="s">
         <v>85</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="23"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="20"/>
+    </row>
+    <row r="19" spans="2:12">
       <c r="B19" s="5">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="6">
         <v>0.02</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="6">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="F19" s="27">
-        <v>0</v>
+      <c r="F19" s="24" t="s">
+        <v>84</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="23"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="20"/>
+    </row>
+    <row r="20" spans="2:12">
       <c r="B20" s="5">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" s="6">
         <v>0.02</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="6">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="F20" s="27">
-        <v>0</v>
+      <c r="F20" s="24" t="s">
+        <v>84</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="23"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L20" s="20"/>
+    </row>
+    <row r="21" spans="2:12">
       <c r="B21" s="5">
         <v>1</v>
       </c>
@@ -1352,12 +1364,12 @@
       <c r="D21" s="6">
         <v>3.85</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="6">
         <f t="shared" si="0"/>
         <v>3.85</v>
       </c>
-      <c r="F21" s="27">
-        <v>9</v>
+      <c r="F21" s="24">
+        <v>14</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>43</v>
@@ -1368,9 +1380,9 @@
       <c r="K21" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L21" s="23"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L21" s="20"/>
+    </row>
+    <row r="22" spans="2:12">
       <c r="B22" s="5">
         <v>1</v>
       </c>
@@ -1380,12 +1392,12 @@
       <c r="D22" s="6">
         <v>0.8</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="6">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="F22" s="27">
-        <v>11</v>
+      <c r="F22" s="24">
+        <v>19</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>44</v>
@@ -1396,9 +1408,9 @@
       <c r="K22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L22" s="23"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L22" s="20"/>
+    </row>
+    <row r="23" spans="2:12">
       <c r="B23" s="5">
         <v>1</v>
       </c>
@@ -1408,12 +1420,12 @@
       <c r="D23" s="6">
         <v>0.1</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="6">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F23" s="27" t="s">
-        <v>85</v>
+      <c r="F23" s="24">
+        <v>65</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>58</v>
@@ -1422,11 +1434,11 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="19" t="s">
+      <c r="L23" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12">
       <c r="B24" s="5">
         <v>1</v>
       </c>
@@ -1436,12 +1448,12 @@
       <c r="D24" s="6">
         <v>0.06</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="6">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="F24" s="27" t="s">
-        <v>85</v>
+      <c r="F24" s="24">
+        <v>69</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>60</v>
@@ -1450,11 +1462,11 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="19" t="s">
+      <c r="L24" s="16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12">
       <c r="B25" s="5">
         <v>2</v>
       </c>
@@ -1464,12 +1476,12 @@
       <c r="D25" s="6">
         <v>0.1</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="6">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="F25" s="27" t="s">
-        <v>85</v>
+      <c r="F25" s="24">
+        <v>129</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>69</v>
@@ -1478,173 +1490,208 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="22"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="5">
-        <v>1</v>
-      </c>
+      <c r="L25" s="19"/>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26" s="5"/>
       <c r="C26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E26" s="1">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="24">
+        <v>8</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="22"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="5">
-        <v>3</v>
-      </c>
+      <c r="L26" s="19"/>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27" s="5"/>
       <c r="C27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="6">
-        <v>0.04</v>
-      </c>
-      <c r="E27" s="1">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-      <c r="F27" s="27">
-        <v>35</v>
+        <v>88</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="24">
+        <v>6</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="5">
-        <v>1</v>
-      </c>
+      <c r="L27" s="19"/>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="B28" s="5"/>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D28" s="6">
-        <f>27.54/50</f>
-        <v>0.55079999999999996</v>
-      </c>
-      <c r="E28" s="1">
-        <f t="shared" si="0"/>
-        <v>0.55079999999999996</v>
-      </c>
-      <c r="F28" s="27">
-        <v>25</v>
+        <v>0.2</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="24">
+        <v>5</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L28" s="19"/>
+    </row>
+    <row r="29" spans="2:12">
       <c r="B29" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="D29" s="6">
-        <v>0.74</v>
-      </c>
-      <c r="E29" s="1">
-        <f>D29*B29</f>
-        <v>0.74</v>
-      </c>
-      <c r="F29" s="27">
-        <v>15</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>0.04</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="6">
+        <f>27.54/50</f>
+        <v>0.55079999999999996</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="0"/>
+        <v>0.55079999999999996</v>
+      </c>
+      <c r="F30" s="24">
+        <v>3</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.74</v>
+      </c>
+      <c r="E31" s="6">
+        <f>D31*B31</f>
+        <v>0.74</v>
+      </c>
+      <c r="F31" s="24">
+        <v>3</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K29" s="4"/>
-      <c r="L29" s="19" t="s">
+      <c r="K31" s="4"/>
+      <c r="L31" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="8"/>
-      <c r="C30" s="9" t="s">
+    <row r="32" spans="2:12" ht="15.75" thickBot="1">
+      <c r="C32" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D32" s="27">
         <v>14.95</v>
       </c>
-      <c r="E30" s="11">
-        <f>D31*B30</f>
+      <c r="E32" s="27">
+        <f>D33*B33</f>
         <v>0</v>
       </c>
-      <c r="F30" s="28">
-        <v>0</v>
-      </c>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15" t="s">
+      <c r="F32" s="25">
+        <v>13</v>
+      </c>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="K30" s="15"/>
-      <c r="L30" s="9"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E31" s="1">
-        <f>SUM(E4:E30)</f>
-        <v>76.463799999999978</v>
-      </c>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="K32" s="12"/>
+      <c r="L32" s="8"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B33" s="7">
+        <f>SUM(B4:B30)</f>
+        <v>38</v>
+      </c>
+      <c r="E33" s="6">
+        <f>SUM(E4:E32)</f>
+        <v>76.263799999999975</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="3" t="s">
+    <row r="35" spans="2:6">
+      <c r="C35" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="3" t="s">
+    <row r="36" spans="2:6">
+      <c r="C36" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="3" t="s">
+    <row r="37" spans="2:6">
+      <c r="C37" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="3" t="s">
+    <row r="38" spans="2:6">
+      <c r="C38" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" s="3" t="s">
+    <row r="39" spans="2:6">
+      <c r="C39" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>